<commit_message>
add bootstrap project and dashboard updates
</commit_message>
<xml_diff>
--- a/Dashboard/CM Techno Schema.xlsx
+++ b/Dashboard/CM Techno Schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKHLZ\Desktop\projects\cm-techno\Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\cm-techno\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46206D09-5B8B-459E-BB26-1119BA046F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47191F8-1089-4E96-A0AB-583A9E852A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="course" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="classroom" sheetId="8" r:id="rId3"/>
     <sheet name="teacher" sheetId="5" r:id="rId4"/>
     <sheet name="ledger" sheetId="9" r:id="rId5"/>
-    <sheet name="student" sheetId="4" r:id="rId6"/>
-    <sheet name="lead" sheetId="6" r:id="rId7"/>
-    <sheet name="attendance" sheetId="3" r:id="rId8"/>
+    <sheet name="installments" sheetId="10" r:id="rId6"/>
+    <sheet name="student" sheetId="4" r:id="rId7"/>
+    <sheet name="lead" sheetId="6" r:id="rId8"/>
+    <sheet name="attendance" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">lead!$A$1:$N$1001</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ledger!$A$1:$L$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">lead!$A$1:$N$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ledger!$A$1:$K$24</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8306" uniqueCount="1762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8449" uniqueCount="1777">
   <si>
     <t>SHORT</t>
   </si>
@@ -5240,9 +5241,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>MBA</t>
   </si>
   <si>
@@ -5327,7 +5325,55 @@
     <t>Python</t>
   </si>
   <si>
-    <t>Prajakta</t>
+    <t>Ishika</t>
+  </si>
+  <si>
+    <t>Kandhari</t>
+  </si>
+  <si>
+    <t>Enrolled</t>
+  </si>
+  <si>
+    <t>qualification</t>
+  </si>
+  <si>
+    <t>age_group</t>
+  </si>
+  <si>
+    <t>Manav</t>
+  </si>
+  <si>
+    <t>Simran</t>
+  </si>
+  <si>
+    <t>Aisha</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>Harsh</t>
+  </si>
+  <si>
+    <t>Aarohi</t>
+  </si>
+  <si>
+    <t>Mahi</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>Atharv</t>
+  </si>
+  <si>
+    <t>Suhani</t>
+  </si>
+  <si>
+    <t>Aadhya</t>
+  </si>
+  <si>
+    <t>Mukherjee</t>
   </si>
 </sst>
 </file>
@@ -5369,7 +5415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5403,25 +5449,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5468,6 +5514,9 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5487,16 +5536,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5513,6 +5553,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5520,6 +5564,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5570,48 +5617,45 @@
     <tableColumn id="8" xr3:uid="{EBDEA6C8-0548-4DBF-B3A3-C0F42E98A724}" name="highest_qualification"/>
     <tableColumn id="9" xr3:uid="{851A0F20-F799-4124-8267-4BBF2C1E0A0B}" name="degree"/>
     <tableColumn id="10" xr3:uid="{927A1A45-3C2B-4100-B02D-35037065DC6E}" name="experience"/>
-    <tableColumn id="11" xr3:uid="{0BA6576C-DEEE-48E4-B04F-DEE5EE4B5CAA}" name="join_date" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{0BA6576C-DEEE-48E4-B04F-DEE5EE4B5CAA}" name="join_date" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{074CBD85-A70F-400A-AB45-1504C0093046}" name="ledger" displayName="ledger" ref="A1:L21" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:L21" xr:uid="{B893101D-DD0E-4D7B-A4CB-6CBFB8C973D2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
-    <sortCondition ref="D1:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{074CBD85-A70F-400A-AB45-1504C0093046}" name="ledger" displayName="ledger" ref="A1:K24" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:K24" xr:uid="{074CBD85-A70F-400A-AB45-1504C0093046}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K24">
+    <sortCondition ref="C1:C24"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{CF45C688-CC45-4B6D-9880-B21C5727C6A8}" name="student_id" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1A50F633-BFAF-43F3-8C78-2E279254CE7B}" name="join_date" dataDxfId="1">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{C0AA2F1D-ABC5-4031-8177-2A1D3CAD388F}" name="total_fee" dataDxfId="4">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{CF45C688-CC45-4B6D-9880-B21C5727C6A8}" name="student_id" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{C0AA2F1D-ABC5-4031-8177-2A1D3CAD388F}" name="total_fee" dataDxfId="24">
       <calculatedColumnFormula>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9B38B735-1F90-4261-8F6B-3B801393DD94}" name="payment_date" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{62AA783A-DF8E-40D5-9E2C-11C619E8D0E3}" name="invoice_no" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{76F42F03-CF09-4B62-A869-EFE7E72482AC}" name="payment_method" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{92C49AE3-EF6C-4EB3-BA02-965369D8DA59}" name="paid_amount" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{7525E932-4BAE-4995-8B30-20E31175CB4D}" name="cumulative_paid" dataDxfId="21">
-      <calculatedColumnFormula>SUMIFS($G:$G,$A:$A,$A2,$D:$D,"&lt;="&amp;$D2)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{9B38B735-1F90-4261-8F6B-3B801393DD94}" name="payment_date" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{62AA783A-DF8E-40D5-9E2C-11C619E8D0E3}" name="invoice_no" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{76F42F03-CF09-4B62-A869-EFE7E72482AC}" name="payment_method" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{92C49AE3-EF6C-4EB3-BA02-965369D8DA59}" name="paid_amount" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{7525E932-4BAE-4995-8B30-20E31175CB4D}" name="cumulative_paid" dataDxfId="1">
+      <calculatedColumnFormula>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B5C3EDF7-C3F0-41AE-8BCE-5F2B006B5CF7}" name="outstanding_amount" dataDxfId="20">
-      <calculatedColumnFormula>$C2-$H2</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{B5C3EDF7-C3F0-41AE-8BCE-5F2B006B5CF7}" name="outstanding_amount" dataDxfId="19">
+      <calculatedColumnFormula>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F8EC42AB-FD39-40C5-A9FE-1CAFDE57DA3D}" name="next_installment_date" dataDxfId="19">
-      <calculatedColumnFormula>IF($I2&gt;0,$D2+30,"")</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{F8EC42AB-FD39-40C5-A9FE-1CAFDE57DA3D}" name="next_installment_date" dataDxfId="3">
+      <calculatedColumnFormula>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4C989DD0-0906-427D-87D7-07D2C23BD79F}" name="next_installment_amount" dataDxfId="18">
-      <calculatedColumnFormula>IF($I2&gt;0,$I2/2,"0")</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{4C989DD0-0906-427D-87D7-07D2C23BD79F}" name="next_installment_amount" dataDxfId="2">
+      <calculatedColumnFormula>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B7145B8F-C136-4E15-9F91-6F3B2702FA99}" name="payment_status" dataDxfId="3">
-      <calculatedColumnFormula>IF(ledger[[#This Row],[cumulative_paid]]=0,
+    <tableColumn id="12" xr3:uid="{B7145B8F-C136-4E15-9F91-6F3B2702FA99}" name="payment_status" dataDxfId="0">
+      <calculatedColumnFormula>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</calculatedColumnFormula>
+      "Paid"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5619,25 +5663,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C48AB8AA-486A-4934-93BB-FAAD4065A993}" name="student" displayName="student" ref="A1:M22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:M22" xr:uid="{C48AB8AA-486A-4934-93BB-FAAD4065A993}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C48AB8AA-486A-4934-93BB-FAAD4065A993}" name="student" displayName="student" ref="A1:N41" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:N41" xr:uid="{C48AB8AA-486A-4934-93BB-FAAD4065A993}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M20">
     <sortCondition ref="A1:A20"/>
   </sortState>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{5D7BAA88-0806-4E45-B0AA-491E00692674}" name="id" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{B263BBE1-98B2-4BC7-858E-30F15F520CE0}" name="year_joined" dataDxfId="2"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{5D7BAA88-0806-4E45-B0AA-491E00692674}" name="id" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{B263BBE1-98B2-4BC7-858E-30F15F520CE0}" name="year_joined" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{1B331B7C-494A-46BC-BA9F-967DA79FB498}" name="first_name" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{E5FF3772-724A-4DA4-AF12-81278BBF4168}" name="last_name" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{607AFD25-D550-42CA-9493-0EF9E8F70B14}" name="join_date" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{BE1D48E6-3762-4E05-AC88-C93CE44E4FC2}" name="course_id" dataDxfId="11"/>
     <tableColumn id="6" xr3:uid="{189ABD32-ED6F-4D29-BA75-EBF2D6B7DD9F}" name="dob" dataDxfId="10"/>
     <tableColumn id="7" xr3:uid="{3D99CBC8-AD3F-4DB4-A77C-75BA0D954B66}" name="gender" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{41697462-FF0D-453D-9B92-8C87261505B7}" name="course" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{41697462-FF0D-453D-9B92-8C87261505B7}" name="qualification" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{D4E60B8E-280C-4D16-98E4-32AC16FF6CA5}" name="class_id" dataDxfId="7"/>
     <tableColumn id="10" xr3:uid="{6C2CD91A-6D0E-4886-A1E6-049820D40F65}" name="status" dataDxfId="6"/>
     <tableColumn id="14" xr3:uid="{907DD65C-0AD6-4218-B0C2-A275A62851D8}" name="certificate_generated" dataDxfId="5"/>
     <tableColumn id="11" xr3:uid="{5B900A8C-B714-416B-ADCF-BAB50AE3B319}" name="total_fee"/>
+    <tableColumn id="12" xr3:uid="{B5138BBE-A6C3-4609-B1E5-8595D95D9DBD}" name="age_group" dataDxfId="4">
+      <calculatedColumnFormula>IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5970,7 +6021,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6331,7 +6382,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -6433,7 +6484,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6706,1050 +6757,1104 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B893101D-DD0E-4D7B-A4CB-6CBFB8C973D2}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.21875" customWidth="1"/>
-    <col min="10" max="10" width="22.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="D1" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="E1" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>41</v>
+        <v>1757</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>1758</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>1757</v>
-      </c>
-      <c r="J1" s="12" t="s">
+        <v>1756</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>1716</v>
       </c>
+      <c r="J1" s="11" t="s">
+        <v>1717</v>
+      </c>
       <c r="K1" s="11" t="s">
-        <v>1717</v>
-      </c>
-      <c r="L1" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>619</v>
       </c>
-      <c r="B2" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>44826</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
         <v>110000</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C2" s="4">
         <v>44788</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>27</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F2" s="3">
+        <v>110000</v>
+      </c>
       <c r="G2" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
         <v>110000</v>
       </c>
       <c r="H2" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A2,$D:$D,"&lt;="&amp;$D2)</f>
-        <v>110000</v>
-      </c>
-      <c r="I2" s="3">
-        <f>$C2-$H2</f>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="str">
-        <f>IF($I2&gt;0,$D2+30,"")</f>
-        <v/>
+      <c r="I2" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>44818</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
       </c>
       <c r="K2" s="3" t="str">
-        <f>IF($I2&gt;0,$I2/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>394</v>
       </c>
-      <c r="B3" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>44787</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
         <v>80000</v>
       </c>
-      <c r="D3" s="4">
+      <c r="C3" s="4">
         <v>44793</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>45</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F3" s="3">
+        <v>80000</v>
+      </c>
       <c r="G3" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
         <v>80000</v>
       </c>
       <c r="H3" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A3,$D:$D,"&lt;="&amp;$D3)</f>
-        <v>80000</v>
-      </c>
-      <c r="I3" s="3">
-        <f>$C3-$H3</f>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
         <v>0</v>
       </c>
-      <c r="J3" s="4" t="str">
-        <f>IF($I3&gt;0,$D3+30,"")</f>
-        <v/>
+      <c r="I3" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>44823</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
       </c>
       <c r="K3" s="3" t="str">
-        <f>IF($I3&gt;0,$I3/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>981</v>
       </c>
-      <c r="B4" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>44933</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
         <v>85000</v>
       </c>
-      <c r="D4" s="4">
+      <c r="C4" s="4">
         <v>45053</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F4" s="3">
+        <v>85000</v>
+      </c>
       <c r="G4" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
         <v>85000</v>
       </c>
       <c r="H4" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A4,$D:$D,"&lt;="&amp;$D4)</f>
-        <v>85000</v>
-      </c>
-      <c r="I4" s="3">
-        <f>$C4-$H4</f>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
         <v>0</v>
       </c>
-      <c r="J4" s="4" t="str">
-        <f>IF($I4&gt;0,$D4+30,"")</f>
-        <v/>
+      <c r="I4" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45083</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
       </c>
       <c r="K4" s="3" t="str">
-        <f>IF($I4&gt;0,$I4/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>553</v>
       </c>
-      <c r="B5" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45258</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
         <v>135000</v>
       </c>
-      <c r="D5" s="4">
+      <c r="C5" s="4">
         <v>45058</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>56</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>1724</v>
       </c>
+      <c r="F5" s="3">
+        <v>135000</v>
+      </c>
       <c r="G5" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
         <v>135000</v>
       </c>
       <c r="H5" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A5,$D:$D,"&lt;="&amp;$D5)</f>
-        <v>135000</v>
-      </c>
-      <c r="I5" s="3">
-        <f>$C5-$H5</f>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
         <v>0</v>
       </c>
-      <c r="J5" s="4" t="str">
-        <f>IF($I5&gt;0,$D5+30,"")</f>
-        <v/>
+      <c r="I5" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45088</v>
+      </c>
+      <c r="J5" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
       </c>
       <c r="K5" s="3" t="str">
-        <f>IF($I5&gt;0,$I5/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>491</v>
       </c>
-      <c r="B6" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45134</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
         <v>100000</v>
       </c>
-      <c r="D6" s="4">
+      <c r="C6" s="4">
         <v>45134</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F6" s="3">
+        <v>50000</v>
+      </c>
       <c r="G6" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
         <v>50000</v>
       </c>
       <c r="H6" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A6,$D:$D,"&lt;="&amp;$D6)</f>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
         <v>50000</v>
       </c>
-      <c r="I6" s="3">
-        <f>$C6-$H6</f>
-        <v>50000</v>
-      </c>
-      <c r="J6" s="4">
-        <f>IF($I6&gt;0,$D6+30,"")</f>
+      <c r="I6" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
         <v>45164</v>
       </c>
-      <c r="K6" s="3">
-        <f>IF($I6&gt;0,$I6/2,"0")</f>
+      <c r="J6" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
         <v>25000</v>
       </c>
-      <c r="L6" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+      <c r="K6" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>513</v>
-      </c>
-      <c r="B7" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45178</v>
-      </c>
-      <c r="C7" s="3">
+        <v>491</v>
+      </c>
+      <c r="B7" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>130000</v>
-      </c>
-      <c r="D7" s="4">
-        <v>45178</v>
-      </c>
-      <c r="E7" s="3">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>45165</v>
+      </c>
+      <c r="D7" s="3">
+        <v>201</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>1726</v>
       </c>
+      <c r="F7" s="3">
+        <v>50000</v>
+      </c>
       <c r="G7" s="3">
-        <v>60000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>100000</v>
       </c>
       <c r="H7" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A7,$D:$D,"&lt;="&amp;$D7)</f>
-        <v>60000</v>
-      </c>
-      <c r="I7" s="3">
-        <f>$C7-$H7</f>
-        <v>70000</v>
-      </c>
-      <c r="J7" s="4">
-        <f>IF($I7&gt;0,$D7+30,"")</f>
-        <v>45208</v>
-      </c>
-      <c r="K7" s="3">
-        <f>IF($I7&gt;0,$I7/2,"0")</f>
-        <v>35000</v>
-      </c>
-      <c r="L7" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45195</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Partially Paid</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>476</v>
-      </c>
-      <c r="B8" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45240</v>
-      </c>
-      <c r="C8" s="3">
+        <v>513</v>
+      </c>
+      <c r="B8" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>85000</v>
-      </c>
-      <c r="D8" s="4">
-        <v>45214</v>
-      </c>
-      <c r="E8" s="3">
-        <v>42</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>1727</v>
+        <v>130000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>45178</v>
+      </c>
+      <c r="D8" s="3">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F8" s="3">
+        <v>60000</v>
       </c>
       <c r="G8" s="3">
-        <v>85000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>60000</v>
       </c>
       <c r="H8" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A8,$D:$D,"&lt;="&amp;$D8)</f>
-        <v>85000</v>
-      </c>
-      <c r="I8" s="3">
-        <f>$C8-$H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="4" t="str">
-        <f>IF($I8&gt;0,$D8+30,"")</f>
-        <v/>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>70000</v>
+      </c>
+      <c r="I8" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45208</v>
+      </c>
+      <c r="J8" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>35000</v>
       </c>
       <c r="K8" s="3" t="str">
-        <f>IF($I8&gt;0,$I8/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Partially Paid</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>658</v>
-      </c>
-      <c r="B9" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45594</v>
-      </c>
-      <c r="C9" s="3">
+        <v>476</v>
+      </c>
+      <c r="B9" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>95000</v>
-      </c>
-      <c r="D9" s="4">
-        <v>45302</v>
-      </c>
-      <c r="E9" s="3">
-        <v>55</v>
-      </c>
-      <c r="F9" s="3" t="s">
+        <v>85000</v>
+      </c>
+      <c r="C9" s="4">
+        <v>45214</v>
+      </c>
+      <c r="D9" s="3">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F9" s="3">
+        <v>85000</v>
+      </c>
       <c r="G9" s="3">
-        <v>95000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>85000</v>
       </c>
       <c r="H9" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A9,$D:$D,"&lt;="&amp;$D9)</f>
-        <v>95000</v>
-      </c>
-      <c r="I9" s="3">
-        <f>$C9-$H9</f>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
         <v>0</v>
       </c>
-      <c r="J9" s="4" t="str">
-        <f>IF($I9&gt;0,$D9+30,"")</f>
-        <v/>
+      <c r="I9" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45244</v>
+      </c>
+      <c r="J9" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
       </c>
       <c r="K9" s="3" t="str">
-        <f>IF($I9&gt;0,$I9/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>736</v>
-      </c>
-      <c r="B10" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45512</v>
-      </c>
-      <c r="C10" s="3">
+        <v>658</v>
+      </c>
+      <c r="B10" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>120000</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45512</v>
-      </c>
-      <c r="E10" s="3">
-        <v>71</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>1724</v>
+        <v>95000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>45302</v>
+      </c>
+      <c r="D10" s="3">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F10" s="3">
+        <v>95000</v>
       </c>
       <c r="G10" s="3">
-        <v>40000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>95000</v>
       </c>
       <c r="H10" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A10,$D:$D,"&lt;="&amp;$D10)</f>
-        <v>40000</v>
-      </c>
-      <c r="I10" s="3">
-        <f>$C10-$H10</f>
-        <v>80000</v>
-      </c>
-      <c r="J10" s="4">
-        <f>IF($I10&gt;0,$D10+30,"")</f>
-        <v>45542</v>
-      </c>
-      <c r="K10" s="3">
-        <f>IF($I10&gt;0,$I10/2,"0")</f>
-        <v>40000</v>
-      </c>
-      <c r="L10" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45332</v>
+      </c>
+      <c r="J10" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Partially Paid</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>827</v>
-      </c>
-      <c r="B11" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45482</v>
-      </c>
-      <c r="C11" s="3">
+        <v>736</v>
+      </c>
+      <c r="B11" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>140000</v>
-      </c>
-      <c r="D11" s="4">
-        <v>45574</v>
-      </c>
-      <c r="E11" s="3">
-        <v>37</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>1725</v>
+        <v>120000</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45512</v>
+      </c>
+      <c r="D11" s="3">
+        <v>71</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F11" s="3">
+        <v>40000</v>
       </c>
       <c r="G11" s="3">
-        <v>140000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>40000</v>
       </c>
       <c r="H11" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A11,$D:$D,"&lt;="&amp;$D11)</f>
-        <v>140000</v>
-      </c>
-      <c r="I11" s="3">
-        <f>$C11-$H11</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4" t="str">
-        <f>IF($I11&gt;0,$D11+30,"")</f>
-        <v/>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>80000</v>
+      </c>
+      <c r="I11" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45542</v>
+      </c>
+      <c r="J11" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>40000</v>
       </c>
       <c r="K11" s="3" t="str">
-        <f>IF($I11&gt;0,$I11/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Partially Paid</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>742</v>
-      </c>
-      <c r="B12" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45585</v>
-      </c>
-      <c r="C12" s="3">
+        <v>827</v>
+      </c>
+      <c r="B12" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>95000</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45585</v>
-      </c>
-      <c r="E12" s="3">
-        <v>91</v>
-      </c>
-      <c r="F12" s="3" t="s">
+        <v>140000</v>
+      </c>
+      <c r="C12" s="4">
+        <v>45574</v>
+      </c>
+      <c r="D12" s="3">
+        <v>37</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>1725</v>
       </c>
+      <c r="F12" s="3">
+        <v>140000</v>
+      </c>
       <c r="G12" s="3">
-        <v>45000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>140000</v>
       </c>
       <c r="H12" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A12,$D:$D,"&lt;="&amp;$D12)</f>
-        <v>45000</v>
-      </c>
-      <c r="I12" s="3">
-        <f>$C12-$H12</f>
-        <v>50000</v>
-      </c>
-      <c r="J12" s="4">
-        <f>IF($I12&gt;0,$D12+30,"")</f>
-        <v>45615</v>
-      </c>
-      <c r="K12" s="3">
-        <f>IF($I12&gt;0,$I12/2,"0")</f>
-        <v>25000</v>
-      </c>
-      <c r="L12" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45604</v>
+      </c>
+      <c r="J12" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Partially Paid</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>227</v>
-      </c>
-      <c r="B13" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
+        <v>742</v>
+      </c>
+      <c r="B13" s="3">
+        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
+        <v>95000</v>
+      </c>
+      <c r="C13" s="4">
+        <v>45585</v>
+      </c>
+      <c r="D13" s="3">
+        <v>91</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F13" s="3">
+        <v>45000</v>
+      </c>
+      <c r="G13" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>45000</v>
+      </c>
+      <c r="H13" s="3">
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>50000</v>
+      </c>
+      <c r="I13" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
         <v>45615</v>
       </c>
-      <c r="C13" s="3">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>150000</v>
-      </c>
-      <c r="D13" s="4">
-        <v>45618</v>
-      </c>
-      <c r="E13" s="3">
-        <v>66</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="G13" s="3">
-        <v>60000</v>
-      </c>
-      <c r="H13" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A13,$D:$D,"&lt;="&amp;$D13)</f>
-        <v>60000</v>
-      </c>
-      <c r="I13" s="3">
-        <f>$C13-$H13</f>
-        <v>90000</v>
-      </c>
-      <c r="J13" s="4">
-        <f>IF($I13&gt;0,$D13+30,"")</f>
-        <v>45648</v>
-      </c>
-      <c r="K13" s="3">
-        <f>IF($I13&gt;0,$I13/2,"0")</f>
-        <v>45000</v>
-      </c>
-      <c r="L13" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+      <c r="J13" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>25000</v>
+      </c>
+      <c r="K13" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>284</v>
-      </c>
-      <c r="B14" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45728</v>
-      </c>
-      <c r="C14" s="3">
+        <v>227</v>
+      </c>
+      <c r="B14" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>125000</v>
-      </c>
-      <c r="D14" s="4">
-        <v>45728</v>
-      </c>
-      <c r="E14" s="3">
-        <v>88</v>
-      </c>
-      <c r="F14" s="3" t="s">
+        <v>150000</v>
+      </c>
+      <c r="C14" s="4">
+        <v>45618</v>
+      </c>
+      <c r="D14" s="3">
+        <v>66</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>1725</v>
       </c>
+      <c r="F14" s="3">
+        <v>60000</v>
+      </c>
       <c r="G14" s="3">
-        <v>30000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>60000</v>
       </c>
       <c r="H14" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A14,$D:$D,"&lt;="&amp;$D14)</f>
-        <v>30000</v>
-      </c>
-      <c r="I14" s="3">
-        <f>$C14-$H14</f>
-        <v>95000</v>
-      </c>
-      <c r="J14" s="4">
-        <f>IF($I14&gt;0,$D14+30,"")</f>
-        <v>45758</v>
-      </c>
-      <c r="K14" s="3">
-        <f>IF($I14&gt;0,$I14/2,"0")</f>
-        <v>47500</v>
-      </c>
-      <c r="L14" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>90000</v>
+      </c>
+      <c r="I14" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45648</v>
+      </c>
+      <c r="J14" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>45000</v>
+      </c>
+      <c r="K14" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>182</v>
-      </c>
-      <c r="B15" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45787</v>
-      </c>
-      <c r="C15" s="3">
+        <v>284</v>
+      </c>
+      <c r="B15" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>120000</v>
-      </c>
-      <c r="D15" s="4">
-        <v>45787</v>
-      </c>
-      <c r="E15" s="3">
-        <v>34</v>
-      </c>
-      <c r="F15" s="3" t="s">
+        <v>125000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>45728</v>
+      </c>
+      <c r="D15" s="3">
+        <v>88</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>1725</v>
       </c>
+      <c r="F15" s="3">
+        <v>30000</v>
+      </c>
       <c r="G15" s="3">
-        <v>40000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>30000</v>
       </c>
       <c r="H15" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A15,$D:$D,"&lt;="&amp;$D15)</f>
-        <v>40000</v>
-      </c>
-      <c r="I15" s="3">
-        <f>$C15-$H15</f>
-        <v>80000</v>
-      </c>
-      <c r="J15" s="4">
-        <f>IF($I15&gt;0,$D15+30,"")</f>
-        <v>45817</v>
-      </c>
-      <c r="K15" s="3">
-        <f>IF($I15&gt;0,$I15/2,"0")</f>
-        <v>40000</v>
-      </c>
-      <c r="L15" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>95000</v>
+      </c>
+      <c r="I15" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45758</v>
+      </c>
+      <c r="J15" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>47500</v>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>392</v>
-      </c>
-      <c r="B16" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45856</v>
-      </c>
-      <c r="C16" s="3">
+        <v>182</v>
+      </c>
+      <c r="B16" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>90000</v>
-      </c>
-      <c r="D16" s="4">
-        <v>45856</v>
-      </c>
-      <c r="E16" s="3">
-        <v>64</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>1726</v>
+        <v>120000</v>
+      </c>
+      <c r="C16" s="4">
+        <v>45787</v>
+      </c>
+      <c r="D16" s="3">
+        <v>34</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F16" s="3">
+        <v>40000</v>
       </c>
       <c r="G16" s="3">
-        <v>30000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>40000</v>
       </c>
       <c r="H16" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A16,$D:$D,"&lt;="&amp;$D16)</f>
-        <v>30000</v>
-      </c>
-      <c r="I16" s="3">
-        <f>$C16-$H16</f>
-        <v>60000</v>
-      </c>
-      <c r="J16" s="4">
-        <f>IF($I16&gt;0,$D16+30,"")</f>
-        <v>45886</v>
-      </c>
-      <c r="K16" s="3">
-        <f>IF($I16&gt;0,$I16/2,"0")</f>
-        <v>30000</v>
-      </c>
-      <c r="L16" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>80000</v>
+      </c>
+      <c r="I16" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45817</v>
+      </c>
+      <c r="J16" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>40000</v>
+      </c>
+      <c r="K16" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>763</v>
-      </c>
-      <c r="B17" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45851</v>
-      </c>
-      <c r="C17" s="3">
+        <v>392</v>
+      </c>
+      <c r="B17" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>150000</v>
-      </c>
-      <c r="D17" s="4">
-        <v>45858</v>
-      </c>
-      <c r="E17" s="3">
-        <v>78</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>1724</v>
+        <v>90000</v>
+      </c>
+      <c r="C17" s="4">
+        <v>45856</v>
+      </c>
+      <c r="D17" s="3">
+        <v>64</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F17" s="3">
+        <v>30000</v>
       </c>
       <c r="G17" s="3">
-        <v>150000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>30000</v>
       </c>
       <c r="H17" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A17,$D:$D,"&lt;="&amp;$D17)</f>
-        <v>150000</v>
-      </c>
-      <c r="I17" s="3">
-        <f>$C17-$H17</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="4" t="str">
-        <f>IF($I17&gt;0,$D17+30,"")</f>
-        <v/>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>60000</v>
+      </c>
+      <c r="I17" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45886</v>
+      </c>
+      <c r="J17" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>30000</v>
       </c>
       <c r="K17" s="3" t="str">
-        <f>IF($I17&gt;0,$I17/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Partially Paid</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>392</v>
-      </c>
-      <c r="B18" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45856</v>
-      </c>
-      <c r="C18" s="3">
+        <v>763</v>
+      </c>
+      <c r="B18" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>90000</v>
-      </c>
-      <c r="D18" s="4">
-        <v>45887</v>
-      </c>
-      <c r="E18" s="3">
-        <v>100</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>1727</v>
+        <v>150000</v>
+      </c>
+      <c r="C18" s="4">
+        <v>45858</v>
+      </c>
+      <c r="D18" s="3">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F18" s="3">
+        <v>150000</v>
       </c>
       <c r="G18" s="3">
-        <v>10000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>150000</v>
       </c>
       <c r="H18" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A18,$D:$D,"&lt;="&amp;$D18)</f>
-        <v>40000</v>
-      </c>
-      <c r="I18" s="3">
-        <f>$C18-$H18</f>
-        <v>50000</v>
-      </c>
-      <c r="J18" s="4">
-        <f>IF($I18&gt;0,$D18+30,"")</f>
-        <v>45917</v>
-      </c>
-      <c r="K18" s="3">
-        <f>IF($I18&gt;0,$I18/2,"0")</f>
-        <v>25000</v>
-      </c>
-      <c r="L18" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45888</v>
+      </c>
+      <c r="J18" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Partially Paid</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      "Paid"))</f>
+        <v>Paid</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>392</v>
       </c>
-      <c r="B19" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45856</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B19" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
         <v>90000</v>
       </c>
-      <c r="D19" s="4">
-        <v>45918</v>
-      </c>
-      <c r="E19" s="3">
-        <v>150</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="C19" s="4">
+        <v>45887</v>
+      </c>
+      <c r="D19" s="3">
+        <v>100</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F19" s="3">
+        <v>10000</v>
+      </c>
       <c r="G19" s="3">
-        <v>30000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>40000</v>
       </c>
       <c r="H19" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A19,$D:$D,"&lt;="&amp;$D19)</f>
-        <v>70000</v>
-      </c>
-      <c r="I19" s="3">
-        <f>$C19-$H19</f>
-        <v>20000</v>
-      </c>
-      <c r="J19" s="4">
-        <f>IF($I19&gt;0,$D19+30,"")</f>
-        <v>45948</v>
-      </c>
-      <c r="K19" s="3">
-        <f>IF($I19&gt;0,$I19/2,"0")</f>
-        <v>10000</v>
-      </c>
-      <c r="L19" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>50000</v>
+      </c>
+      <c r="I19" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45917</v>
+      </c>
+      <c r="J19" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>25000</v>
+      </c>
+      <c r="K19" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>835</v>
-      </c>
-      <c r="B20" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45925</v>
-      </c>
-      <c r="C20" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B20" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>90000</v>
-      </c>
-      <c r="D20" s="4">
-        <v>45925</v>
-      </c>
-      <c r="E20" s="3">
-        <v>99</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>1724</v>
+        <v>50000</v>
+      </c>
+      <c r="C20" s="4">
+        <v>45889</v>
+      </c>
+      <c r="D20" s="3">
+        <v>200</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F20" s="3">
+        <v>25000</v>
       </c>
       <c r="G20" s="3">
-        <v>30000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>25000</v>
       </c>
       <c r="H20" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A20,$D:$D,"&lt;="&amp;$D20)</f>
-        <v>30000</v>
-      </c>
-      <c r="I20" s="3">
-        <f>$C20-$H20</f>
-        <v>60000</v>
-      </c>
-      <c r="J20" s="4">
-        <f>IF($I20&gt;0,$D20+30,"")</f>
-        <v>45955</v>
-      </c>
-      <c r="K20" s="3">
-        <f>IF($I20&gt;0,$I20/2,"0")</f>
-        <v>30000</v>
-      </c>
-      <c r="L20" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>25000</v>
+      </c>
+      <c r="I20" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45919</v>
+      </c>
+      <c r="J20" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>12500</v>
+      </c>
+      <c r="K20" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
+      "Paid"))</f>
         <v>Partially Paid</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>392</v>
-      </c>
-      <c r="B21" s="1">
-        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[join_date], "Not Found")</f>
-        <v>45856</v>
-      </c>
-      <c r="C21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="3">
         <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
-        <v>90000</v>
-      </c>
-      <c r="D21" s="4">
-        <v>45948</v>
-      </c>
-      <c r="E21" s="3">
-        <v>160</v>
-      </c>
-      <c r="F21" s="3" t="s">
+        <v>50000</v>
+      </c>
+      <c r="C21" s="4">
+        <v>45894</v>
+      </c>
+      <c r="D21" s="3">
+        <v>201</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>1727</v>
       </c>
+      <c r="F21" s="3">
+        <v>12500</v>
+      </c>
       <c r="G21" s="3">
-        <v>20000</v>
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>37500</v>
       </c>
       <c r="H21" s="3">
-        <f>SUMIFS($G:$G,$A:$A,$A21,$D:$D,"&lt;="&amp;$D21)</f>
-        <v>90000</v>
-      </c>
-      <c r="I21" s="3">
-        <f>$C21-$H21</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="4" t="str">
-        <f>IF($I21&gt;0,$D21+30,"")</f>
-        <v/>
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>12500</v>
+      </c>
+      <c r="I21" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45924</v>
+      </c>
+      <c r="J21" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>6250</v>
       </c>
       <c r="K21" s="3" t="str">
-        <f>IF($I21&gt;0,$I21/2,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="3" t="str">
-        <f>IF(ledger[[#This Row],[cumulative_paid]]=0,
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
    "Not Paid",
    IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
       "Partially Paid",
-      "Cleared"))</f>
-        <v>Cleared</v>
+      "Paid"))</f>
+        <v>Partially Paid</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>392</v>
+      </c>
+      <c r="B22" s="3">
+        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
+        <v>90000</v>
+      </c>
+      <c r="C22" s="4">
+        <v>45918</v>
+      </c>
+      <c r="D22" s="3">
+        <v>150</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F22" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G22" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>70000</v>
+      </c>
+      <c r="H22" s="3">
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>20000</v>
+      </c>
+      <c r="I22" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45948</v>
+      </c>
+      <c r="J22" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>10000</v>
+      </c>
+      <c r="K22" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
+   "Not Paid",
+   IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
+      "Partially Paid",
+      "Paid"))</f>
+        <v>Partially Paid</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>835</v>
+      </c>
+      <c r="B23" s="3">
+        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
+        <v>90000</v>
+      </c>
+      <c r="C23" s="4">
+        <v>45925</v>
+      </c>
+      <c r="D23" s="3">
+        <v>99</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F23" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G23" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>30000</v>
+      </c>
+      <c r="H23" s="3">
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>60000</v>
+      </c>
+      <c r="I23" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45955</v>
+      </c>
+      <c r="J23" s="3">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>30000</v>
+      </c>
+      <c r="K23" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
+   "Not Paid",
+   IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
+      "Partially Paid",
+      "Paid"))</f>
+        <v>Partially Paid</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>392</v>
+      </c>
+      <c r="B24" s="3">
+        <f>_xlfn.XLOOKUP(ledger[[#This Row],[student_id]], student[id], student[total_fee], "Not Found")</f>
+        <v>90000</v>
+      </c>
+      <c r="C24" s="4">
+        <v>45948</v>
+      </c>
+      <c r="D24" s="3">
+        <v>160</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F24" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G24" s="3">
+        <f>SUMIFS(ledger[paid_amount],ledger[student_id],ledger[[#This Row],[student_id]],ledger[payment_date], "&lt;=" &amp;ledger[[#This Row],[payment_date]])</f>
+        <v>90000</v>
+      </c>
+      <c r="H24" s="3">
+        <f>ledger[[#This Row],[total_fee]] - ledger[[#This Row],[cumulative_paid]]</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <f>IF(ledger[[#This Row],[payment_date]] &gt; 0,ledger[[#This Row],[payment_date]] + 30, "")</f>
+        <v>45978</v>
+      </c>
+      <c r="J24" s="3" t="str">
+        <f>IF(ledger[[#This Row],[outstanding_amount]] &gt; 0,ledger[[#This Row],[outstanding_amount]] / 2, "0")</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="3" t="str">
+        <f>IF(ledger[[#This Row],[cumulative_paid]] = 0,
+   "Not Paid",
+   IF(ledger[[#This Row],[cumulative_paid]]&lt;ledger[[#This Row],[total_fee]],
+      "Partially Paid",
+      "Paid"))</f>
+        <v>Paid</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{A8496351-B6BC-4B5D-B69C-AAB818B27F0C}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{A8496351-B6BC-4B5D-B69C-AAB818B27F0C}">
       <formula1>"Cash, NEFT, UPI, Credit Card"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K24" xr:uid="{1C22B42C-5652-44C5-93B1-0F60C3155687}">
+      <formula1>"Paid, Partially Paid, Refunded, Overdue, Overpaid, Absoconded"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7760,11 +7865,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F792792-6AA3-4E84-903B-17E1D8698F83}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7774,22 +7893,23 @@
     <col min="3" max="3" width="12.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="9.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" style="3" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>25</v>
@@ -7801,7 +7921,7 @@
         <v>76</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>36</v>
@@ -7810,7 +7930,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>77</v>
+        <v>1763</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>38</v>
@@ -7819,13 +7939,16 @@
         <v>34</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="6" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>182</v>
       </c>
@@ -7854,19 +7977,27 @@
         <v>171</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L2" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M2">
         <v>120000</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>190</v>
       </c>
@@ -7895,19 +8026,27 @@
         <v>171</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L3" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M3">
         <v>120000</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>227</v>
       </c>
@@ -7915,7 +8054,7 @@
         <v>2024</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1240</v>
@@ -7933,22 +8072,30 @@
         <v>1729</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L4" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="M4">
         <v>150000</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>284</v>
       </c>
@@ -7959,7 +8106,7 @@
         <v>194</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="E5" s="5">
         <v>45728</v>
@@ -7974,22 +8121,30 @@
         <v>1729</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L5" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M5">
         <v>125000</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>392</v>
       </c>
@@ -7997,10 +8152,10 @@
         <v>2025</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>1746</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>1747</v>
       </c>
       <c r="E6" s="5">
         <v>45856</v>
@@ -8018,19 +8173,27 @@
         <v>87</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L6" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M6">
         <v>90000</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>394</v>
       </c>
@@ -8038,7 +8201,7 @@
         <v>2022</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>329</v>
@@ -8056,22 +8219,30 @@
         <v>1731</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L7" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="M7">
         <v>80000</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>476</v>
       </c>
@@ -8079,7 +8250,7 @@
         <v>2023</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1306</v>
@@ -8097,22 +8268,30 @@
         <v>1731</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L8" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M8">
         <v>85000</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>491</v>
       </c>
@@ -8120,7 +8299,7 @@
         <v>2023</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>601</v>
@@ -8141,19 +8320,27 @@
         <v>87</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L9" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M9">
         <v>100000</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>513</v>
       </c>
@@ -8161,10 +8348,10 @@
         <v>2023</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>1734</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1735</v>
       </c>
       <c r="E10" s="5">
         <v>45178</v>
@@ -8179,22 +8366,30 @@
         <v>1731</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L10" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M10">
         <v>130000</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>553</v>
       </c>
@@ -8202,7 +8397,7 @@
         <v>2023</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>440</v>
@@ -8223,19 +8418,27 @@
         <v>171</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L11" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M11">
         <v>135000</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>619</v>
       </c>
@@ -8243,7 +8446,7 @@
         <v>2022</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>1283</v>
@@ -8264,19 +8467,27 @@
         <v>103</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L12" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M12">
         <v>110000</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>625</v>
       </c>
@@ -8284,7 +8495,7 @@
         <v>2022</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>1555</v>
@@ -8305,19 +8516,27 @@
         <v>103</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L13" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="M13">
         <v>110000</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>658</v>
       </c>
@@ -8346,19 +8565,27 @@
         <v>87</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L14" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M14">
         <v>95000</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>736</v>
       </c>
@@ -8369,7 +8596,7 @@
         <v>472</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="E15" s="5">
         <v>45512</v>
@@ -8387,19 +8614,27 @@
         <v>171</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L15" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M15">
         <v>120000</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>742</v>
       </c>
@@ -8407,10 +8642,10 @@
         <v>2024</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>1750</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>1751</v>
       </c>
       <c r="E16" s="5">
         <v>45585</v>
@@ -8425,22 +8660,30 @@
         <v>1729</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L16" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M16">
         <v>95000</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>763</v>
       </c>
@@ -8466,22 +8709,30 @@
         <v>1729</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L17" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M17">
         <v>150000</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>827</v>
       </c>
@@ -8489,7 +8740,7 @@
         <v>2024</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>529</v>
@@ -8507,22 +8758,30 @@
         <v>1729</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L18" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="M18">
         <v>140000</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>835</v>
       </c>
@@ -8551,19 +8810,27 @@
         <v>103</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L19" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M19">
         <v>90000</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>981</v>
       </c>
@@ -8592,19 +8859,27 @@
         <v>103</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>1730</v>
       </c>
       <c r="L20" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="M20">
         <v>85000</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>1000</v>
       </c>
@@ -8612,19 +8887,19 @@
         <v>2025</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>1761</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>928</v>
-      </c>
       <c r="E21" s="5">
-        <v>45879</v>
-      </c>
-      <c r="F21" s="13">
+        <v>45889</v>
+      </c>
+      <c r="F21" s="10">
         <v>6</v>
       </c>
       <c r="G21" s="4">
-        <v>38752</v>
+        <v>38387</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>1729</v>
@@ -8633,16 +8908,1004 @@
         <v>87</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>1732</v>
+        <v>1762</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="M21">
         <v>50000</v>
+      </c>
+      <c r="N21" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>1001</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E22" s="5">
+        <v>45029</v>
+      </c>
+      <c r="F22" s="10">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>36874</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M22">
+        <v>125000</v>
+      </c>
+      <c r="N22" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>1002</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E23" s="5">
+        <v>44832</v>
+      </c>
+      <c r="F23" s="10">
+        <v>4</v>
+      </c>
+      <c r="G23" s="4">
+        <v>36267</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M23">
+        <v>155000</v>
+      </c>
+      <c r="N23" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>1003</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="E24" s="5">
+        <v>45363</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>38541</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M24">
+        <v>110000</v>
+      </c>
+      <c r="N24" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>1004</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="E25" s="5">
+        <v>44947</v>
+      </c>
+      <c r="F25" s="10">
+        <v>7</v>
+      </c>
+      <c r="G25" s="4">
+        <v>38089</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M25">
+        <v>110000</v>
+      </c>
+      <c r="N25" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1005</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E26" s="5">
+        <v>45779</v>
+      </c>
+      <c r="F26" s="10">
+        <v>7</v>
+      </c>
+      <c r="G26" s="4">
+        <v>39297</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M26">
+        <v>150000</v>
+      </c>
+      <c r="N26" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>1006</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E27" s="5">
+        <v>45988</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
+        <v>37344</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M27">
+        <v>115000</v>
+      </c>
+      <c r="N27" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>1007</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="E28" s="5">
+        <v>45391</v>
+      </c>
+      <c r="F28" s="10">
+        <v>6</v>
+      </c>
+      <c r="G28" s="4">
+        <v>38346</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M28">
+        <v>85000</v>
+      </c>
+      <c r="N28" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>1008</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E29" s="5">
+        <v>45078</v>
+      </c>
+      <c r="F29" s="10">
+        <v>4</v>
+      </c>
+      <c r="G29" s="4">
+        <v>38848</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M29">
+        <v>155000</v>
+      </c>
+      <c r="N29" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>1009</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1768</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="E30" s="5">
+        <v>45807</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>36469</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="M30">
+        <v>105000</v>
+      </c>
+      <c r="N30" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>1010</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="5">
+        <v>45549</v>
+      </c>
+      <c r="F31" s="10">
+        <v>8</v>
+      </c>
+      <c r="G31" s="4">
+        <v>39061</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M31">
+        <v>115000</v>
+      </c>
+      <c r="N31" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>1011</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="E32" s="5">
+        <v>45585</v>
+      </c>
+      <c r="F32" s="10">
+        <v>7</v>
+      </c>
+      <c r="G32" s="4">
+        <v>38544</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M32">
+        <v>120000</v>
+      </c>
+      <c r="N32" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>1012</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="5">
+        <v>44838</v>
+      </c>
+      <c r="F33" s="10">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4">
+        <v>37052</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="M33">
+        <v>80000</v>
+      </c>
+      <c r="N33" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>1013</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="E34" s="5">
+        <v>45971</v>
+      </c>
+      <c r="F34" s="10">
+        <v>9</v>
+      </c>
+      <c r="G34" s="4">
+        <v>39104</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="M34">
+        <v>80000</v>
+      </c>
+      <c r="N34" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>1014</v>
+      </c>
+      <c r="B35" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E35" s="5">
+        <v>45544</v>
+      </c>
+      <c r="F35" s="10">
+        <v>5</v>
+      </c>
+      <c r="G35" s="4">
+        <v>37127</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M35">
+        <v>90000</v>
+      </c>
+      <c r="N35" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>1015</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E36" s="5">
+        <v>46002</v>
+      </c>
+      <c r="F36" s="10">
+        <v>5</v>
+      </c>
+      <c r="G36" s="4">
+        <v>39131</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="M36">
+        <v>80000</v>
+      </c>
+      <c r="N36" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>1016</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="E37" s="5">
+        <v>45350</v>
+      </c>
+      <c r="F37" s="10">
+        <v>2</v>
+      </c>
+      <c r="G37" s="4">
+        <v>37791</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M37">
+        <v>90000</v>
+      </c>
+      <c r="N37" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>1017</v>
+      </c>
+      <c r="B38" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>1772</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E38" s="5">
+        <v>45479</v>
+      </c>
+      <c r="F38" s="10">
+        <v>2</v>
+      </c>
+      <c r="G38" s="4">
+        <v>37162</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M38">
+        <v>105000</v>
+      </c>
+      <c r="N38" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>1018</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E39" s="5">
+        <v>45847</v>
+      </c>
+      <c r="F39" s="10">
+        <v>7</v>
+      </c>
+      <c r="G39" s="4">
+        <v>39257</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M39">
+        <v>130000</v>
+      </c>
+      <c r="N39" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>Below 20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>1019</v>
+      </c>
+      <c r="B40" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1774</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E40" s="5">
+        <v>45342</v>
+      </c>
+      <c r="F40" s="10">
+        <v>9</v>
+      </c>
+      <c r="G40" s="4">
+        <v>36889</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M40">
+        <v>80000</v>
+      </c>
+      <c r="N40" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>1020</v>
+      </c>
+      <c r="B41" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1776</v>
+      </c>
+      <c r="E41" s="5">
+        <v>45346</v>
+      </c>
+      <c r="F41" s="10">
+        <v>4</v>
+      </c>
+      <c r="G41" s="4">
+        <v>36769</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="M41">
+        <v>125000</v>
+      </c>
+      <c r="N41" s="3" t="str">
+        <f ca="1">IF(student[[#This Row],[dob]]="","",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;20,"Below 20",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;30,"20 to 29",
+IF(DATEDIF(student[[#This Row],[dob]],TODAY(),"y")&lt;40,"30 to 39",
+"Above 40"))))</f>
+        <v>20 to 29</v>
       </c>
     </row>
   </sheetData>
@@ -8654,29 +9917,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A975" workbookViewId="0">
+      <selection activeCell="D986" sqref="D986"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -43731,12 +44995,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>